<commit_message>
Updated report and transparency improvement
</commit_message>
<xml_diff>
--- a/Analysis/v4 Output Excel/ggppa_progressivity_results_v4.xlsx
+++ b/Analysis/v4 Output Excel/ggppa_progressivity_results_v4.xlsx
@@ -15,7 +15,7 @@
   <sheets>
     <sheet name="ggppa_progressivity_results_v4" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" calcCompleted="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -1276,10 +1276,10 @@
   <dimension ref="A1:AV141"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="U2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Y6" sqref="Y6"/>
+      <selection pane="bottomRight" activeCell="X7" sqref="X7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>